<commit_message>
Finishing code for saving_data. Outputting data and creating folder for completed data sets
</commit_message>
<xml_diff>
--- a/Saving_Data.xlsx
+++ b/Saving_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\Documents\GitHub\ISYS40251_Deriving-Value-Data-Analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E234C5E-9B1C-4194-81B7-500DB71C77FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5FD4E7-4C62-41A9-9A74-BA8E3D08E62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Monthly Saving (£)</t>
+  </si>
+  <si>
+    <t>Saving Target (£)</t>
   </si>
   <si>
     <t>Jan 2022</t>
@@ -146,9 +149,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -198,12 +198,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,18 +505,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,509 +533,620 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>216706</v>
+        <v>213799</v>
       </c>
       <c r="C2">
-        <v>209002</v>
-      </c>
-      <c r="D2" s="2">
-        <v>7704</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>201172</v>
+      </c>
+      <c r="D2">
+        <v>12627</v>
+      </c>
+      <c r="E2">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>215217</v>
+        <v>217526</v>
       </c>
       <c r="C3">
-        <v>209091</v>
-      </c>
-      <c r="D3" s="2">
-        <v>6126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>209025</v>
+      </c>
+      <c r="D3">
+        <v>8501</v>
+      </c>
+      <c r="E3">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>252603</v>
+        <v>207863</v>
       </c>
       <c r="C4">
-        <v>237372</v>
-      </c>
-      <c r="D4" s="2">
-        <v>15231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>189602</v>
+      </c>
+      <c r="D4">
+        <v>18261</v>
+      </c>
+      <c r="E4">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>273675</v>
+        <v>207299</v>
       </c>
       <c r="C5">
-        <v>253188</v>
-      </c>
-      <c r="D5" s="2">
-        <v>20487</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>185378</v>
+      </c>
+      <c r="D5">
+        <v>21921</v>
+      </c>
+      <c r="E5">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>202066</v>
+        <v>225065</v>
       </c>
       <c r="C6">
-        <v>187031</v>
-      </c>
-      <c r="D6" s="2">
-        <v>15035</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>195479</v>
+      </c>
+      <c r="D6">
+        <v>29586</v>
+      </c>
+      <c r="E6">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>217871</v>
+        <v>261948</v>
       </c>
       <c r="C7">
-        <v>207782</v>
-      </c>
-      <c r="D7" s="2">
-        <v>10089</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>243025</v>
+      </c>
+      <c r="D7">
+        <v>18923</v>
+      </c>
+      <c r="E7">
+        <v>15750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>219252</v>
+        <v>240539</v>
       </c>
       <c r="C8">
-        <v>201326</v>
-      </c>
-      <c r="D8" s="2">
-        <v>17926</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>225829</v>
+      </c>
+      <c r="D8">
+        <v>14710</v>
+      </c>
+      <c r="E8">
+        <v>16800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>202125</v>
+        <v>213868</v>
       </c>
       <c r="C9">
-        <v>185464</v>
-      </c>
-      <c r="D9" s="2">
-        <v>16661</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>205691</v>
+      </c>
+      <c r="D9">
+        <v>8177</v>
+      </c>
+      <c r="E9">
+        <v>18450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>209542</v>
+        <v>200727</v>
       </c>
       <c r="C10">
-        <v>185984</v>
-      </c>
-      <c r="D10" s="2">
-        <v>23558</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>188073</v>
+      </c>
+      <c r="D10">
+        <v>12654</v>
+      </c>
+      <c r="E10">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>200989</v>
+        <v>217317</v>
       </c>
       <c r="C11">
-        <v>189474</v>
-      </c>
-      <c r="D11" s="2">
-        <v>11515</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>206040</v>
+      </c>
+      <c r="D11">
+        <v>11277</v>
+      </c>
+      <c r="E11">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>200262</v>
+        <v>250936</v>
       </c>
       <c r="C12">
-        <v>188196</v>
-      </c>
-      <c r="D12" s="2">
-        <v>12066</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>243158</v>
+      </c>
+      <c r="D12">
+        <v>7778</v>
+      </c>
+      <c r="E12">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13">
-        <v>200859</v>
+        <v>207367</v>
       </c>
       <c r="C13">
-        <v>187758</v>
-      </c>
-      <c r="D13" s="2">
-        <v>13101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>186096</v>
+      </c>
+      <c r="D13">
+        <v>21271</v>
+      </c>
+      <c r="E13">
+        <v>25500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>200876</v>
+        <v>208944</v>
       </c>
       <c r="C14">
-        <v>187618</v>
-      </c>
-      <c r="D14" s="2">
-        <v>13258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>185364</v>
+      </c>
+      <c r="D14">
+        <v>23580</v>
+      </c>
+      <c r="E14">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>200096</v>
+        <v>208832</v>
       </c>
       <c r="C15">
-        <v>186780</v>
-      </c>
-      <c r="D15" s="2">
-        <v>13316</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>187036</v>
+      </c>
+      <c r="D15">
+        <v>21796</v>
+      </c>
+      <c r="E15">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>206017</v>
+        <v>239127</v>
       </c>
       <c r="C16">
-        <v>188512</v>
-      </c>
-      <c r="D16" s="2">
-        <v>17505</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>229166</v>
+      </c>
+      <c r="D16">
+        <v>9961</v>
+      </c>
+      <c r="E16">
+        <v>11500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17">
-        <v>200715</v>
+        <v>210804</v>
       </c>
       <c r="C17">
-        <v>185052</v>
-      </c>
-      <c r="D17" s="2">
-        <v>15663</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>205133</v>
+      </c>
+      <c r="D17">
+        <v>5671</v>
+      </c>
+      <c r="E17">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18">
-        <v>202438</v>
+        <v>204878</v>
       </c>
       <c r="C18">
-        <v>187009</v>
-      </c>
-      <c r="D18" s="2">
-        <v>15429</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>187577</v>
+      </c>
+      <c r="D18">
+        <v>17301</v>
+      </c>
+      <c r="E18">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19">
-        <v>204799</v>
+        <v>214620</v>
       </c>
       <c r="C19">
-        <v>189674</v>
-      </c>
-      <c r="D19" s="2">
-        <v>15125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>204173</v>
+      </c>
+      <c r="D19">
+        <v>10447</v>
+      </c>
+      <c r="E19">
+        <v>16750</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20">
-        <v>202470</v>
+        <v>218002</v>
       </c>
       <c r="C20">
-        <v>189807</v>
-      </c>
-      <c r="D20" s="2">
-        <v>12663</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>200011</v>
+      </c>
+      <c r="D20">
+        <v>17991</v>
+      </c>
+      <c r="E20">
+        <v>17800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21">
-        <v>202357</v>
+        <v>205158</v>
       </c>
       <c r="C21">
-        <v>186323</v>
-      </c>
-      <c r="D21" s="2">
-        <v>16034</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>189865</v>
+      </c>
+      <c r="D21">
+        <v>15293</v>
+      </c>
+      <c r="E21">
+        <v>19450</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22">
-        <v>220954</v>
+        <v>281309</v>
       </c>
       <c r="C22">
-        <v>199149</v>
-      </c>
-      <c r="D22" s="2">
-        <v>21805</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>253678</v>
+      </c>
+      <c r="D22">
+        <v>27631</v>
+      </c>
+      <c r="E22">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23">
-        <v>212380</v>
+        <v>211647</v>
       </c>
       <c r="C23">
-        <v>207101</v>
-      </c>
-      <c r="D23" s="2">
-        <v>5279</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>207582</v>
+      </c>
+      <c r="D23">
+        <v>4065</v>
+      </c>
+      <c r="E23">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24">
-        <v>215710</v>
+        <v>202771</v>
       </c>
       <c r="C24">
-        <v>207267</v>
-      </c>
-      <c r="D24" s="2">
-        <v>8443</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>189246</v>
+      </c>
+      <c r="D24">
+        <v>13525</v>
+      </c>
+      <c r="E24">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25">
-        <v>208658</v>
+        <v>218711</v>
       </c>
       <c r="C25">
-        <v>188670</v>
-      </c>
-      <c r="D25" s="2">
-        <v>19988</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>209094</v>
+      </c>
+      <c r="D25">
+        <v>9617</v>
+      </c>
+      <c r="E25">
+        <v>26500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26">
-        <v>232213</v>
+        <v>213221</v>
       </c>
       <c r="C26">
-        <v>211314</v>
-      </c>
-      <c r="D26" s="2">
-        <v>20899</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>205902</v>
+      </c>
+      <c r="D26">
+        <v>7319</v>
+      </c>
+      <c r="E26">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27">
-        <v>210227</v>
+        <v>220935</v>
       </c>
       <c r="C27">
-        <v>206133</v>
-      </c>
-      <c r="D27" s="2">
-        <v>4094</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>205747</v>
+      </c>
+      <c r="D27">
+        <v>15188</v>
+      </c>
+      <c r="E27">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28">
-        <v>252290</v>
+        <v>200069</v>
       </c>
       <c r="C28">
-        <v>244650</v>
-      </c>
-      <c r="D28" s="2">
-        <v>7640</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>185625</v>
+      </c>
+      <c r="D28">
+        <v>14444</v>
+      </c>
+      <c r="E28">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29">
-        <v>200819</v>
+        <v>213960</v>
       </c>
       <c r="C29">
-        <v>186125</v>
-      </c>
-      <c r="D29" s="2">
-        <v>14694</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>208646</v>
+      </c>
+      <c r="D29">
+        <v>5314</v>
+      </c>
+      <c r="E29">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30">
-        <v>215944</v>
+        <v>211922</v>
       </c>
       <c r="C30">
-        <v>185989</v>
-      </c>
-      <c r="D30" s="2">
-        <v>29955</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>204324</v>
+      </c>
+      <c r="D30">
+        <v>7598</v>
+      </c>
+      <c r="E30">
+        <v>15500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31">
-        <v>217859</v>
+        <v>202087</v>
       </c>
       <c r="C31">
-        <v>208466</v>
-      </c>
-      <c r="D31" s="2">
-        <v>9393</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>186653</v>
+      </c>
+      <c r="D31">
+        <v>15434</v>
+      </c>
+      <c r="E31">
+        <v>17250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32">
-        <v>212723</v>
+        <v>207901</v>
       </c>
       <c r="C32">
-        <v>200053</v>
-      </c>
-      <c r="D32" s="2">
-        <v>12670</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>188926</v>
+      </c>
+      <c r="D32">
+        <v>18975</v>
+      </c>
+      <c r="E32">
+        <v>18300</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33">
-        <v>209323</v>
+        <v>216175</v>
       </c>
       <c r="C33">
-        <v>189966</v>
-      </c>
-      <c r="D33" s="2">
-        <v>19357</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>200372</v>
+      </c>
+      <c r="D33">
+        <v>15803</v>
+      </c>
+      <c r="E33">
+        <v>19950</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34">
-        <v>273342</v>
+        <v>209407</v>
       </c>
       <c r="C34">
-        <v>245376</v>
-      </c>
-      <c r="D34" s="2">
-        <v>27966</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>185122</v>
+      </c>
+      <c r="D34">
+        <v>24285</v>
+      </c>
+      <c r="E34">
+        <v>20500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35">
-        <v>209809</v>
+        <v>202097</v>
       </c>
       <c r="C35">
-        <v>185987</v>
-      </c>
-      <c r="D35" s="2">
-        <v>23822</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>180505</v>
+      </c>
+      <c r="D35">
+        <v>21592</v>
+      </c>
+      <c r="E35">
+        <v>23500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36">
-        <v>211267</v>
+        <v>211218</v>
       </c>
       <c r="C36">
-        <v>208156</v>
-      </c>
-      <c r="D36" s="2">
-        <v>3111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>203022</v>
+      </c>
+      <c r="D36">
+        <v>8196</v>
+      </c>
+      <c r="E36">
+        <v>25500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37">
-        <v>264625</v>
+        <v>203684</v>
       </c>
       <c r="C37">
-        <v>246249</v>
-      </c>
-      <c r="D37" s="2">
-        <v>18376</v>
+        <v>185587</v>
+      </c>
+      <c r="D37">
+        <v>18097</v>
+      </c>
+      <c r="E37">
+        <v>27000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>